<commit_message>
zeitblatt aktualisiert! cc2531 dongel
</commit_message>
<xml_diff>
--- a/Zeitblaetter/Jim Frey.xlsx
+++ b/Zeitblaetter/Jim Frey.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Studium\GitHub_AlienHacky\Zeitblätter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_AlienHacky\Zeitblaetter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="22">
   <si>
     <t>Datum</t>
   </si>
@@ -87,6 +87,15 @@
   </si>
   <si>
     <t xml:space="preserve">I/O Pins geprüft zwischen CC2650 und Senor Hub, Bild erstellt, wie Pins angepasst werden müssen. Konkret I2C  muss anders liegen, wenn Analog kein interrupt hat muss der Lichtsensor Pin umgelegt werden.  Stecker gesucht und flachbandkabel! </t>
+  </si>
+  <si>
+    <t>13.30 - 16.30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Präsentation für Design </t>
+  </si>
+  <si>
+    <t>16.30- 17.30</t>
   </si>
 </sst>
 </file>
@@ -437,10 +446,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C42"/>
+  <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -476,7 +485,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <f>A4+1</f>
         <v>42645</v>
@@ -570,7 +579,7 @@
       </c>
       <c r="B15" s="6"/>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <f t="shared" si="0"/>
         <v>42656</v>
@@ -582,7 +591,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <f t="shared" si="0"/>
         <v>42657</v>
@@ -594,27 +603,27 @@
         <v>11</v>
       </c>
     </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <f t="shared" si="0"/>
         <v>42658</v>
       </c>
       <c r="B18" s="6"/>
     </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <f t="shared" si="0"/>
         <v>42659</v>
       </c>
     </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <f t="shared" si="0"/>
         <v>42660</v>
       </c>
       <c r="B20" s="6"/>
     </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <f t="shared" si="0"/>
         <v>42661</v>
@@ -626,7 +635,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="1">
         <f t="shared" si="0"/>
         <v>42662</v>
@@ -638,7 +647,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="1">
         <f t="shared" si="0"/>
         <v>42663</v>
@@ -650,7 +659,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="1">
         <f t="shared" si="0"/>
         <v>42664</v>
@@ -662,7 +671,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="1">
         <f t="shared" si="0"/>
         <v>42665</v>
@@ -674,7 +683,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="1">
         <f t="shared" si="0"/>
         <v>42666</v>
@@ -686,14 +695,14 @@
         <v>17</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>42667</v>
       </c>
       <c r="B27" s="6"/>
     </row>
-    <row r="28" spans="1:3" ht="63" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="63" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
         <f t="shared" si="0"/>
         <v>42668</v>
@@ -705,28 +714,39 @@
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="1">
         <f t="shared" si="0"/>
         <v>42669</v>
       </c>
-      <c r="B29" s="6"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29" s="6">
+        <v>4</v>
+      </c>
+      <c r="C29" t="s">
+        <v>20</v>
+      </c>
+      <c r="D29" t="s">
+        <v>19</v>
+      </c>
+      <c r="E29" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>42670</v>
       </c>
       <c r="B30" s="6"/>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>42671</v>
       </c>
       <c r="B31" s="6"/>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>42672</v>
@@ -757,7 +777,7 @@
       </c>
       <c r="B36" s="8">
         <f>SUM(B5:B34)</f>
-        <v>31.7</v>
+        <v>35.700000000000003</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Zeitblatt auf stand. I2C Änderungen sind unrelevant
</commit_message>
<xml_diff>
--- a/Zeitblaetter/Jim Frey.xlsx
+++ b/Zeitblaetter/Jim Frey.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eigene Dateien\Documents\Eigene Daten\#Master_3\S1_Kopplung\GitHub_AlienHacky\Zeitblätter\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Git_AlienHacky\Zeitblaetter\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
   <si>
     <t>Datum</t>
   </si>
@@ -84,6 +84,24 @@
   </si>
   <si>
     <t xml:space="preserve">I2C Beispiel geschrieben, gibt fehler beim start der Transaction </t>
+  </si>
+  <si>
+    <t>Teile gesucht um ein prototyp für das Pinmapping zubauen, wie auch nach lesen, prüfen was nicht stimmt</t>
+  </si>
+  <si>
+    <t>Löten der Platine, Kabelbruch im Kabel festgestellt somit alternative überlegt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umlöte, da kein Flachbandkabel verwendet wurde, Test gemacht ohne erfolg bekomme beim Transceive immer 0 zurück </t>
+  </si>
+  <si>
+    <t>zweiten Prototyp gelötet, die Prototyp fertig gestellt. Idee für befestigung des CC265o mit kleinen adapter Platinen als gummi laschen</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test mit cc2650 i2c zum laufen zu bringen, Recherche in tests ohne erfolg </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Test mit tiva c und cc2650 am osziloskop, CC2650 vermutlich hw fehler </t>
   </si>
 </sst>
 </file>
@@ -437,7 +455,7 @@
   <dimension ref="A1:C42"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+      <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -683,12 +701,17 @@
         <v>16</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A27" s="1">
         <f t="shared" si="0"/>
         <v>42667</v>
       </c>
-      <c r="B27" s="6"/>
+      <c r="B27" s="6">
+        <v>1</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="1">
@@ -703,71 +726,95 @@
         <v>42669</v>
       </c>
       <c r="B29" s="6"/>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A30" s="1">
         <f t="shared" si="0"/>
         <v>42670</v>
       </c>
-      <c r="B30" s="6"/>
+      <c r="B30" s="6">
+        <v>4</v>
+      </c>
+      <c r="C30" s="7" t="s">
+        <v>20</v>
+      </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="1">
         <f t="shared" si="0"/>
         <v>42671</v>
       </c>
-      <c r="B31" s="6"/>
+      <c r="B31" s="6">
+        <v>4</v>
+      </c>
+      <c r="C31" s="7" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="1">
         <f t="shared" si="0"/>
         <v>42672</v>
       </c>
-      <c r="B32" s="6"/>
-    </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B32" s="6">
+        <v>2.5</v>
+      </c>
+      <c r="C32" s="7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A33" s="1">
         <f t="shared" si="0"/>
         <v>42673</v>
       </c>
-      <c r="B33" s="6"/>
-    </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B33" s="6">
+        <v>1</v>
+      </c>
+      <c r="C33" s="7" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="1">
         <f t="shared" si="0"/>
         <v>42674</v>
       </c>
       <c r="B34" s="6"/>
-    </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="C34" s="7"/>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="6"/>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
         <v>3</v>
       </c>
       <c r="B36" s="8">
         <f>SUM(B5:B34)</f>
-        <v>30.2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
+        <v>42.7</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
     </row>
-    <row r="39" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
     </row>
-    <row r="40" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
     </row>
-    <row r="41" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="1"/>
     </row>
-    <row r="42" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="1"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Zeitblatt auf stand gebracht
</commit_message>
<xml_diff>
--- a/Zeitblaetter/Jim Frey.xlsx
+++ b/Zeitblaetter/Jim Frey.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="51195" windowHeight="28260" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="51195" windowHeight="28260" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Oktober" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="26">
   <si>
     <t>Datum</t>
   </si>
@@ -102,6 +102,12 @@
   </si>
   <si>
     <t xml:space="preserve">Test mit tiva c und cc2650 am osziloskop, CC2650 vermutlich hw fehler </t>
+  </si>
+  <si>
+    <t>Zigbee4Java</t>
+  </si>
+  <si>
+    <t>d</t>
   </si>
 </sst>
 </file>
@@ -454,7 +460,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C42"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+    <sheetView topLeftCell="A20" workbookViewId="0">
       <selection activeCell="C32" sqref="C32"/>
     </sheetView>
   </sheetViews>
@@ -827,7 +833,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C36"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
@@ -860,12 +868,21 @@
         <f>A4+1</f>
         <v>42676</v>
       </c>
+      <c r="B5">
+        <v>1</v>
+      </c>
+      <c r="C5" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <f t="shared" ref="A6:A33" si="0">A5+1</f>
         <v>42677</v>
       </c>
+      <c r="C6" t="s">
+        <v>25</v>
+      </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
@@ -1041,7 +1058,7 @@
       </c>
       <c r="B36" s="2">
         <f>SUM(B5:B34)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>